<commit_message>
fix cut offs sheet name error
</commit_message>
<xml_diff>
--- a/src/R/risk_cut_offs.xlsx
+++ b/src/R/risk_cut_offs.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/olivermazariegos/Sites/polio-risk/src/R/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F8D69617-9BFE-204D-9FBE-4F2C0F78B90A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{036FC56F-51D8-1048-8F13-20F67CD053A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1900" yWindow="1820" windowWidth="24500" windowHeight="17240" xr2:uid="{5C1FCA5E-1AE1-4E42-BC50-0F3DA39A67C4}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="sheet_cut_off" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -308,15 +308,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -328,6 +319,15 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -645,7 +645,7 @@
   <dimension ref="A1:E14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+      <selection activeCell="C32" sqref="C32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -725,16 +725,16 @@
     </row>
     <row r="7" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A8" s="8" t="s">
+      <c r="A8" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="B8" s="9"/>
-      <c r="C8" s="9"/>
-      <c r="D8" s="9"/>
-      <c r="E8" s="10"/>
+      <c r="B8" s="16"/>
+      <c r="C8" s="16"/>
+      <c r="D8" s="16"/>
+      <c r="E8" s="17"/>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A9" s="11" t="s">
+      <c r="A9" s="8" t="s">
         <v>0</v>
       </c>
       <c r="B9" s="3" t="s">
@@ -746,60 +746,60 @@
       <c r="D9" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="E9" s="12" t="s">
+      <c r="E9" s="9" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A10" s="13" t="s">
+      <c r="A10" s="10" t="s">
         <v>5</v>
       </c>
       <c r="B10" s="7"/>
       <c r="C10" s="7"/>
       <c r="D10" s="7"/>
-      <c r="E10" s="14"/>
+      <c r="E10" s="11"/>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A11" s="13" t="s">
+      <c r="A11" s="10" t="s">
         <v>6</v>
       </c>
       <c r="B11" s="7"/>
       <c r="C11" s="7"/>
       <c r="D11" s="7"/>
-      <c r="E11" s="14"/>
+      <c r="E11" s="11"/>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A12" s="13" t="s">
+      <c r="A12" s="10" t="s">
         <v>7</v>
       </c>
       <c r="B12" s="7"/>
       <c r="C12" s="7"/>
       <c r="D12" s="7"/>
-      <c r="E12" s="14"/>
+      <c r="E12" s="11"/>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A13" s="13" t="s">
+      <c r="A13" s="10" t="s">
         <v>8</v>
       </c>
       <c r="B13" s="7"/>
       <c r="C13" s="7"/>
       <c r="D13" s="7"/>
-      <c r="E13" s="14"/>
+      <c r="E13" s="11"/>
     </row>
     <row r="14" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="15" t="s">
+      <c r="A14" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="B14" s="16" t="s">
+      <c r="B14" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="C14" s="16" t="s">
+      <c r="C14" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="D14" s="16" t="s">
+      <c r="D14" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="E14" s="17" t="s">
+      <c r="E14" s="14" t="s">
         <v>14</v>
       </c>
     </row>

</xml_diff>

<commit_message>
debugging, still to do
</commit_message>
<xml_diff>
--- a/src/R/risk_cut_offs.xlsx
+++ b/src/R/risk_cut_offs.xlsx
@@ -8,13 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/olivermazariegos/Sites/polio-risk/src/R/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B46629B-D551-EB45-B96C-B7A314760758}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8F4287D-565D-DD48-A18C-B853634DBEEC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1900" yWindow="1820" windowWidth="24500" windowHeight="17240" xr2:uid="{5C1FCA5E-1AE1-4E42-BC50-0F3DA39A67C4}"/>
+    <workbookView xWindow="1900" yWindow="1820" windowWidth="24500" windowHeight="17240" activeTab="1" xr2:uid="{5C1FCA5E-1AE1-4E42-BC50-0F3DA39A67C4}"/>
   </bookViews>
   <sheets>
-    <sheet name="sheet_cut_off" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
+    <sheet name="CUT OFFS" sheetId="1" r:id="rId1"/>
+    <sheet name="sheet_cut_off" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="20">
   <si>
     <t>RV</t>
   </si>
@@ -82,6 +82,21 @@
   </si>
   <si>
     <t>60 &lt; x &lt;= 100</t>
+  </si>
+  <si>
+    <t>immunity_score</t>
+  </si>
+  <si>
+    <t>survaillance_score</t>
+  </si>
+  <si>
+    <t>determinant_score</t>
+  </si>
+  <si>
+    <t>outbreak_score</t>
+  </si>
+  <si>
+    <t>total_score</t>
   </si>
 </sst>
 </file>
@@ -645,7 +660,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F1957B83-55DF-0B40-AC0F-FC36128368F5}">
   <dimension ref="A1:E14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A8" sqref="A8:E8"/>
     </sheetView>
   </sheetViews>
@@ -816,8 +831,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{82FE0BB4-AF07-D248-8277-AD8E94C85802}">
   <dimension ref="A1:E6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C30" sqref="C30"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -844,27 +859,27 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>5</v>
+        <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>6</v>
+        <v>16</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>7</v>
+        <v>17</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>9</v>
+        <v>19</v>
       </c>
       <c r="B6">
         <v>34</v>

</xml_diff>

<commit_message>
value box and filters work
</commit_message>
<xml_diff>
--- a/src/R/risk_cut_offs.xlsx
+++ b/src/R/risk_cut_offs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/olivermazariegos/Sites/polio-risk/src/R/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8F4287D-565D-DD48-A18C-B853634DBEEC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{921D117C-A255-2A45-B676-CF4D72FB2BAD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1900" yWindow="1820" windowWidth="24500" windowHeight="17240" activeTab="1" xr2:uid="{5C1FCA5E-1AE1-4E42-BC50-0F3DA39A67C4}"/>
   </bookViews>
@@ -832,12 +832,12 @@
   <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G17" sqref="G17"/>
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="14.5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
@@ -861,20 +861,68 @@
       <c r="A2" t="s">
         <v>15</v>
       </c>
+      <c r="B2">
+        <v>23</v>
+      </c>
+      <c r="C2">
+        <v>32</v>
+      </c>
+      <c r="D2">
+        <v>39</v>
+      </c>
+      <c r="E2">
+        <v>40</v>
+      </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>16</v>
       </c>
+      <c r="B3">
+        <v>12</v>
+      </c>
+      <c r="C3">
+        <v>17</v>
+      </c>
+      <c r="D3">
+        <v>20</v>
+      </c>
+      <c r="E3">
+        <v>21</v>
+      </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>17</v>
       </c>
+      <c r="B4">
+        <v>0</v>
+      </c>
+      <c r="C4">
+        <v>6</v>
+      </c>
+      <c r="D4">
+        <v>10</v>
+      </c>
+      <c r="E4">
+        <v>11</v>
+      </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>18</v>
+      </c>
+      <c r="B5">
+        <v>2</v>
+      </c>
+      <c r="C5">
+        <v>6</v>
+      </c>
+      <c r="D5">
+        <v>8</v>
+      </c>
+      <c r="E5">
+        <v>9</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
General view for all indicators
</commit_message>
<xml_diff>
--- a/src/R/risk_cut_offs.xlsx
+++ b/src/R/risk_cut_offs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/olivermazariegos/Sites/polio-risk/src/R/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA6726CE-37A9-8247-A13F-BC115E294434}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C326C32-F844-BE4F-BC0E-5C8BDC39A3DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1900" yWindow="1820" windowWidth="24500" windowHeight="17240" activeTab="1" xr2:uid="{5C1FCA5E-1AE1-4E42-BC50-0F3DA39A67C4}"/>
   </bookViews>
@@ -90,13 +90,13 @@
     <t>survaillance_score</t>
   </si>
   <si>
-    <t>determinant_score</t>
-  </si>
-  <si>
-    <t>outbreak_score</t>
-  </si>
-  <si>
     <t>total_score</t>
+  </si>
+  <si>
+    <t>determinants_score</t>
+  </si>
+  <si>
+    <t>outbreaks_score</t>
   </si>
 </sst>
 </file>
@@ -832,7 +832,7 @@
   <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -893,10 +893,10 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B4">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="C4">
         <v>6</v>
@@ -910,7 +910,7 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B5">
         <v>2</v>
@@ -927,7 +927,7 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B6">
         <v>34</v>

</xml_diff>

<commit_message>
adding new cut offs with pfa condition (everything works)
</commit_message>
<xml_diff>
--- a/src/R/risk_cut_offs.xlsx
+++ b/src/R/risk_cut_offs.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/olivermazariegos/Sites/polio-risk/src/R/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C326C32-F844-BE4F-BC0E-5C8BDC39A3DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF3E89A5-125B-AE47-9437-8FBB2BFBFF74}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1900" yWindow="1820" windowWidth="24500" windowHeight="17240" activeTab="1" xr2:uid="{5C1FCA5E-1AE1-4E42-BC50-0F3DA39A67C4}"/>
   </bookViews>
   <sheets>
     <sheet name="CUT OFFS" sheetId="1" r:id="rId1"/>
     <sheet name="sheet_cut_off" sheetId="2" r:id="rId2"/>
+    <sheet name="sheet_cut_off_pfa" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="21">
   <si>
     <t>RV</t>
   </si>
@@ -97,6 +98,9 @@
   </si>
   <si>
     <t>outbreaks_score</t>
+  </si>
+  <si>
+    <t>PFA</t>
   </si>
 </sst>
 </file>
@@ -829,15 +833,242 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{82FE0BB4-AF07-D248-8277-AD8E94C85802}">
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="16.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.83203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B2" t="b">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <v>19</v>
+      </c>
+      <c r="D2">
+        <v>25</v>
+      </c>
+      <c r="E2">
+        <v>32</v>
+      </c>
+      <c r="F2">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B3" t="b">
+        <v>0</v>
+      </c>
+      <c r="C3">
+        <v>24</v>
+      </c>
+      <c r="D3">
+        <v>32</v>
+      </c>
+      <c r="E3">
+        <v>40</v>
+      </c>
+      <c r="F3">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B4" t="b">
+        <v>1</v>
+      </c>
+      <c r="C4">
+        <v>12</v>
+      </c>
+      <c r="D4">
+        <v>16</v>
+      </c>
+      <c r="E4">
+        <v>22</v>
+      </c>
+      <c r="F4">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5" t="b">
+        <v>0</v>
+      </c>
+      <c r="C5">
+        <v>0</v>
+      </c>
+      <c r="D5">
+        <v>8</v>
+      </c>
+      <c r="E5">
+        <v>12</v>
+      </c>
+      <c r="F5">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>18</v>
+      </c>
+      <c r="B6" t="b">
+        <v>1</v>
+      </c>
+      <c r="C6">
+        <v>0</v>
+      </c>
+      <c r="D6">
+        <v>5</v>
+      </c>
+      <c r="E6">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>18</v>
+      </c>
+      <c r="B7" t="b">
+        <v>0</v>
+      </c>
+      <c r="C7">
+        <v>0</v>
+      </c>
+      <c r="D7">
+        <v>6</v>
+      </c>
+      <c r="E7">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>19</v>
+      </c>
+      <c r="B8" t="b">
+        <v>1</v>
+      </c>
+      <c r="C8">
+        <v>0</v>
+      </c>
+      <c r="D8">
+        <v>2</v>
+      </c>
+      <c r="E8">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>19</v>
+      </c>
+      <c r="B9" t="b">
+        <v>0</v>
+      </c>
+      <c r="C9">
+        <v>0</v>
+      </c>
+      <c r="D9">
+        <v>2</v>
+      </c>
+      <c r="E9">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>17</v>
+      </c>
+      <c r="B10" t="b">
+        <v>1</v>
+      </c>
+      <c r="C10">
+        <v>34</v>
+      </c>
+      <c r="D10">
+        <v>48</v>
+      </c>
+      <c r="E10">
+        <v>60</v>
+      </c>
+      <c r="F10">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>17</v>
+      </c>
+      <c r="B11" t="b">
+        <v>0</v>
+      </c>
+      <c r="C11">
+        <v>34</v>
+      </c>
+      <c r="D11">
+        <v>48</v>
+      </c>
+      <c r="E11">
+        <v>60</v>
+      </c>
+      <c r="F11">
+        <v>100</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DBB221D3-86B0-8F45-BCCD-281D04BF6637}">
+  <dimension ref="A1:E6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C29" sqref="C29"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="20.1640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
feat(immunity): total risk points
</commit_message>
<xml_diff>
--- a/src/R/risk_cut_offs.xlsx
+++ b/src/R/risk_cut_offs.xlsx
@@ -8,14 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/olivermazariegos/Sites/polio-risk/src/R/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF3E89A5-125B-AE47-9437-8FBB2BFBFF74}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBA00079-33F0-E843-84A9-C218C8AFDAA4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1900" yWindow="1820" windowWidth="24500" windowHeight="17240" activeTab="1" xr2:uid="{5C1FCA5E-1AE1-4E42-BC50-0F3DA39A67C4}"/>
+    <workbookView xWindow="1900" yWindow="1820" windowWidth="24500" windowHeight="17240" xr2:uid="{5C1FCA5E-1AE1-4E42-BC50-0F3DA39A67C4}"/>
   </bookViews>
   <sheets>
     <sheet name="CUT OFFS" sheetId="1" r:id="rId1"/>
     <sheet name="sheet_cut_off" sheetId="2" r:id="rId2"/>
-    <sheet name="sheet_cut_off_pfa" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -38,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="51">
   <si>
     <t>RV</t>
   </si>
@@ -101,6 +100,96 @@
   </si>
   <si>
     <t>PFA</t>
+  </si>
+  <si>
+    <t>&gt;100000 o con &lt;100000 pero que si haya tenido casos de PFA</t>
+  </si>
+  <si>
+    <t>&lt;100000 que no haya tenido casos de PFA</t>
+  </si>
+  <si>
+    <t>Inmunidad</t>
+  </si>
+  <si>
+    <t>Máximo puntaje</t>
+  </si>
+  <si>
+    <t>Muy alto</t>
+  </si>
+  <si>
+    <t>&gt;=33</t>
+  </si>
+  <si>
+    <t>&gt;=41</t>
+  </si>
+  <si>
+    <t>Alto</t>
+  </si>
+  <si>
+    <t>26-32</t>
+  </si>
+  <si>
+    <t>33-40</t>
+  </si>
+  <si>
+    <t>Medio</t>
+  </si>
+  <si>
+    <t>20-25</t>
+  </si>
+  <si>
+    <t>25-32</t>
+  </si>
+  <si>
+    <t>Bajo</t>
+  </si>
+  <si>
+    <t>&lt;=19</t>
+  </si>
+  <si>
+    <t>&lt;=24</t>
+  </si>
+  <si>
+    <t>Vigilancia</t>
+  </si>
+  <si>
+    <t>&gt;=23</t>
+  </si>
+  <si>
+    <t>17-22</t>
+  </si>
+  <si>
+    <t>13-16</t>
+  </si>
+  <si>
+    <t>&lt;=12</t>
+  </si>
+  <si>
+    <t>Determinantes</t>
+  </si>
+  <si>
+    <t>No aplica</t>
+  </si>
+  <si>
+    <t>Casos y brotes de EPV</t>
+  </si>
+  <si>
+    <t>&gt;=4</t>
+  </si>
+  <si>
+    <t>Total</t>
+  </si>
+  <si>
+    <t>&gt;=61</t>
+  </si>
+  <si>
+    <t>49-60</t>
+  </si>
+  <si>
+    <t>35-48</t>
+  </si>
+  <si>
+    <t>&lt;=34</t>
   </si>
 </sst>
 </file>
@@ -132,7 +221,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -175,8 +264,26 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF5050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="10">
+  <borders count="17">
     <border>
       <left/>
       <right/>
@@ -305,11 +412,106 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="48">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -347,6 +549,82 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -662,10 +940,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F1957B83-55DF-0B40-AC0F-FC36128368F5}">
-  <dimension ref="A1:E14"/>
+  <dimension ref="A1:K40"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A8" sqref="A8:E8"/>
+    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="D30" sqref="D30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -673,7 +951,7 @@
     <col min="1" max="5" width="17.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -690,7 +968,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2" s="7" t="s">
         <v>5</v>
       </c>
@@ -699,7 +977,7 @@
       <c r="D2" s="1"/>
       <c r="E2" s="1"/>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3" s="7" t="s">
         <v>6</v>
       </c>
@@ -708,7 +986,7 @@
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4" s="7" t="s">
         <v>7</v>
       </c>
@@ -717,7 +995,7 @@
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5" s="7" t="s">
         <v>8</v>
       </c>
@@ -726,7 +1004,7 @@
       <c r="D5" s="1"/>
       <c r="E5" s="1"/>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A6" s="7" t="s">
         <v>9</v>
       </c>
@@ -743,8 +1021,8 @@
         <v>61</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:11" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A8" s="15" t="s">
         <v>10</v>
       </c>
@@ -753,7 +1031,7 @@
       <c r="D8" s="16"/>
       <c r="E8" s="17"/>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A9" s="8" t="s">
         <v>0</v>
       </c>
@@ -770,7 +1048,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A10" s="10" t="s">
         <v>5</v>
       </c>
@@ -779,7 +1057,7 @@
       <c r="D10" s="7"/>
       <c r="E10" s="11"/>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A11" s="10" t="s">
         <v>6</v>
       </c>
@@ -788,7 +1066,7 @@
       <c r="D11" s="7"/>
       <c r="E11" s="11"/>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A12" s="10" t="s">
         <v>7</v>
       </c>
@@ -797,7 +1075,7 @@
       <c r="D12" s="7"/>
       <c r="E12" s="11"/>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A13" s="10" t="s">
         <v>8</v>
       </c>
@@ -806,7 +1084,7 @@
       <c r="D13" s="7"/>
       <c r="E13" s="11"/>
     </row>
-    <row r="14" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A14" s="12" t="s">
         <v>9</v>
       </c>
@@ -823,8 +1101,320 @@
         <v>14</v>
       </c>
     </row>
+    <row r="16" spans="1:11" ht="120" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="I16" s="18"/>
+      <c r="J16" s="19" t="s">
+        <v>21</v>
+      </c>
+      <c r="K16" s="19" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="17" spans="8:11" x14ac:dyDescent="0.2">
+      <c r="H17" s="20" t="s">
+        <v>23</v>
+      </c>
+      <c r="I17" s="21" t="s">
+        <v>24</v>
+      </c>
+      <c r="J17" s="22">
+        <v>54</v>
+      </c>
+      <c r="K17" s="23">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="18" spans="8:11" x14ac:dyDescent="0.2">
+      <c r="H18" s="24"/>
+      <c r="I18" s="25" t="s">
+        <v>25</v>
+      </c>
+      <c r="J18" s="26" t="s">
+        <v>26</v>
+      </c>
+      <c r="K18" s="27" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="19" spans="8:11" x14ac:dyDescent="0.2">
+      <c r="H19" s="24"/>
+      <c r="I19" s="28" t="s">
+        <v>28</v>
+      </c>
+      <c r="J19" s="26" t="s">
+        <v>29</v>
+      </c>
+      <c r="K19" s="27" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="20" spans="8:11" x14ac:dyDescent="0.2">
+      <c r="H20" s="24"/>
+      <c r="I20" s="29" t="s">
+        <v>31</v>
+      </c>
+      <c r="J20" s="26" t="s">
+        <v>32</v>
+      </c>
+      <c r="K20" s="27" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="21" spans="8:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="H21" s="30"/>
+      <c r="I21" s="31" t="s">
+        <v>34</v>
+      </c>
+      <c r="J21" s="32" t="s">
+        <v>35</v>
+      </c>
+      <c r="K21" s="33" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="22" spans="8:11" x14ac:dyDescent="0.2">
+      <c r="H22" s="20" t="s">
+        <v>37</v>
+      </c>
+      <c r="I22" s="21" t="s">
+        <v>24</v>
+      </c>
+      <c r="J22" s="22">
+        <v>36</v>
+      </c>
+      <c r="K22" s="23">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="23" spans="8:11" x14ac:dyDescent="0.2">
+      <c r="H23" s="24"/>
+      <c r="I23" s="25" t="s">
+        <v>25</v>
+      </c>
+      <c r="J23" s="26" t="s">
+        <v>38</v>
+      </c>
+      <c r="K23" s="27">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="24" spans="8:11" x14ac:dyDescent="0.2">
+      <c r="H24" s="24"/>
+      <c r="I24" s="28" t="s">
+        <v>28</v>
+      </c>
+      <c r="J24" s="26" t="s">
+        <v>39</v>
+      </c>
+      <c r="K24" s="34">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="25" spans="8:11" x14ac:dyDescent="0.2">
+      <c r="H25" s="24"/>
+      <c r="I25" s="29" t="s">
+        <v>31</v>
+      </c>
+      <c r="J25" s="26" t="s">
+        <v>40</v>
+      </c>
+      <c r="K25" s="34">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="26" spans="8:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="H26" s="30"/>
+      <c r="I26" s="31" t="s">
+        <v>34</v>
+      </c>
+      <c r="J26" s="32" t="s">
+        <v>41</v>
+      </c>
+      <c r="K26" s="33">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="8:11" x14ac:dyDescent="0.2">
+      <c r="H27" s="20" t="s">
+        <v>42</v>
+      </c>
+      <c r="I27" s="21" t="s">
+        <v>24</v>
+      </c>
+      <c r="J27" s="35">
+        <v>10</v>
+      </c>
+      <c r="K27" s="23">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="28" spans="8:11" x14ac:dyDescent="0.2">
+      <c r="H28" s="24"/>
+      <c r="I28" s="25" t="s">
+        <v>25</v>
+      </c>
+      <c r="J28" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="K28" s="27" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="29" spans="8:11" x14ac:dyDescent="0.2">
+      <c r="H29" s="24"/>
+      <c r="I29" s="28" t="s">
+        <v>28</v>
+      </c>
+      <c r="J29" s="36">
+        <v>10</v>
+      </c>
+      <c r="K29" s="37">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="30" spans="8:11" x14ac:dyDescent="0.2">
+      <c r="H30" s="24"/>
+      <c r="I30" s="29" t="s">
+        <v>31</v>
+      </c>
+      <c r="J30" s="36">
+        <v>5</v>
+      </c>
+      <c r="K30" s="37">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="31" spans="8:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="H31" s="30"/>
+      <c r="I31" s="31" t="s">
+        <v>34</v>
+      </c>
+      <c r="J31" s="38">
+        <v>0</v>
+      </c>
+      <c r="K31" s="39">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="8:11" x14ac:dyDescent="0.2">
+      <c r="H32" s="40" t="s">
+        <v>44</v>
+      </c>
+      <c r="I32" s="21" t="s">
+        <v>24</v>
+      </c>
+      <c r="J32" s="35">
+        <v>14</v>
+      </c>
+      <c r="K32" s="41">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="33" spans="8:11" x14ac:dyDescent="0.2">
+      <c r="H33" s="42"/>
+      <c r="I33" s="25" t="s">
+        <v>25</v>
+      </c>
+      <c r="J33" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="K33" s="27" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="34" spans="8:11" x14ac:dyDescent="0.2">
+      <c r="H34" s="42"/>
+      <c r="I34" s="28" t="s">
+        <v>28</v>
+      </c>
+      <c r="J34" s="36" t="s">
+        <v>45</v>
+      </c>
+      <c r="K34" s="37" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="35" spans="8:11" x14ac:dyDescent="0.2">
+      <c r="H35" s="42"/>
+      <c r="I35" s="29" t="s">
+        <v>31</v>
+      </c>
+      <c r="J35" s="36">
+        <v>2</v>
+      </c>
+      <c r="K35" s="37">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="36" spans="8:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="H36" s="43"/>
+      <c r="I36" s="31" t="s">
+        <v>34</v>
+      </c>
+      <c r="J36" s="38">
+        <v>0</v>
+      </c>
+      <c r="K36" s="39">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="8:11" x14ac:dyDescent="0.2">
+      <c r="H37" s="44" t="s">
+        <v>46</v>
+      </c>
+      <c r="I37" s="45" t="s">
+        <v>25</v>
+      </c>
+      <c r="J37" s="35" t="s">
+        <v>47</v>
+      </c>
+      <c r="K37" s="41" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="38" spans="8:11" x14ac:dyDescent="0.2">
+      <c r="H38" s="46"/>
+      <c r="I38" s="28" t="s">
+        <v>28</v>
+      </c>
+      <c r="J38" s="36" t="s">
+        <v>48</v>
+      </c>
+      <c r="K38" s="37" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="39" spans="8:11" x14ac:dyDescent="0.2">
+      <c r="H39" s="46"/>
+      <c r="I39" s="29" t="s">
+        <v>31</v>
+      </c>
+      <c r="J39" s="36" t="s">
+        <v>49</v>
+      </c>
+      <c r="K39" s="37" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="40" spans="8:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="H40" s="47"/>
+      <c r="I40" s="31" t="s">
+        <v>34</v>
+      </c>
+      <c r="J40" s="38" t="s">
+        <v>50</v>
+      </c>
+      <c r="K40" s="39" t="s">
+        <v>50</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="6">
+    <mergeCell ref="H37:H40"/>
+    <mergeCell ref="H17:H21"/>
+    <mergeCell ref="H22:H26"/>
+    <mergeCell ref="H27:H31"/>
+    <mergeCell ref="H32:H36"/>
     <mergeCell ref="A8:E8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -835,7 +1425,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{82FE0BB4-AF07-D248-8277-AD8E94C85802}">
   <dimension ref="A1:F11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
@@ -1056,124 +1646,4 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DBB221D3-86B0-8F45-BCCD-281D04BF6637}">
-  <dimension ref="A1:E6"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C29" sqref="C29"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="20.1640625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>15</v>
-      </c>
-      <c r="B2">
-        <v>23</v>
-      </c>
-      <c r="C2">
-        <v>32</v>
-      </c>
-      <c r="D2">
-        <v>39</v>
-      </c>
-      <c r="E2">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>16</v>
-      </c>
-      <c r="B3">
-        <v>12</v>
-      </c>
-      <c r="C3">
-        <v>17</v>
-      </c>
-      <c r="D3">
-        <v>20</v>
-      </c>
-      <c r="E3">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>18</v>
-      </c>
-      <c r="B4">
-        <v>4</v>
-      </c>
-      <c r="C4">
-        <v>6</v>
-      </c>
-      <c r="D4">
-        <v>10</v>
-      </c>
-      <c r="E4">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>19</v>
-      </c>
-      <c r="B5">
-        <v>2</v>
-      </c>
-      <c r="C5">
-        <v>6</v>
-      </c>
-      <c r="D5">
-        <v>8</v>
-      </c>
-      <c r="E5">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>17</v>
-      </c>
-      <c r="B6">
-        <v>34</v>
-      </c>
-      <c r="C6">
-        <v>48</v>
-      </c>
-      <c r="D6">
-        <v>60</v>
-      </c>
-      <c r="E6">
-        <v>100</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
fix: surveillance for survaillance
</commit_message>
<xml_diff>
--- a/src/R/risk_cut_offs.xlsx
+++ b/src/R/risk_cut_offs.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11008"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11028"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/olivermazariegos/Sites/polio-risk/src/R/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBA00079-33F0-E843-84A9-C218C8AFDAA4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CCDDDDC8-8A2D-4748-9315-CD46F6724E21}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1900" yWindow="1820" windowWidth="24500" windowHeight="17240" xr2:uid="{5C1FCA5E-1AE1-4E42-BC50-0F3DA39A67C4}"/>
+    <workbookView xWindow="1900" yWindow="1820" windowWidth="24500" windowHeight="17240" activeTab="1" xr2:uid="{5C1FCA5E-1AE1-4E42-BC50-0F3DA39A67C4}"/>
   </bookViews>
   <sheets>
     <sheet name="CUT OFFS" sheetId="1" r:id="rId1"/>
@@ -87,9 +87,6 @@
     <t>immunity_score</t>
   </si>
   <si>
-    <t>survaillance_score</t>
-  </si>
-  <si>
     <t>total_score</t>
   </si>
   <si>
@@ -190,6 +187,9 @@
   </si>
   <si>
     <t>&lt;=34</t>
+  </si>
+  <si>
+    <t>surveillance_score</t>
   </si>
 </sst>
 </file>
@@ -541,22 +541,10 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -564,9 +552,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -576,9 +561,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -604,27 +586,45 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -942,7 +942,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F1957B83-55DF-0B40-AC0F-FC36128368F5}">
   <dimension ref="A1:K40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+    <sheetView topLeftCell="A12" workbookViewId="0">
       <selection activeCell="D30" sqref="D30"/>
     </sheetView>
   </sheetViews>
@@ -1023,13 +1023,13 @@
     </row>
     <row r="7" spans="1:11" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="8" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A8" s="15" t="s">
+      <c r="A8" s="45" t="s">
         <v>10</v>
       </c>
-      <c r="B8" s="16"/>
-      <c r="C8" s="16"/>
-      <c r="D8" s="16"/>
-      <c r="E8" s="17"/>
+      <c r="B8" s="46"/>
+      <c r="C8" s="46"/>
+      <c r="D8" s="46"/>
+      <c r="E8" s="47"/>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A9" s="8" t="s">
@@ -1102,320 +1102,320 @@
       </c>
     </row>
     <row r="16" spans="1:11" ht="120" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="I16" s="18"/>
-      <c r="J16" s="19" t="s">
+      <c r="I16" s="15"/>
+      <c r="J16" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="K16" s="16" t="s">
         <v>21</v>
       </c>
-      <c r="K16" s="19" t="s">
+    </row>
+    <row r="17" spans="8:11" x14ac:dyDescent="0.2">
+      <c r="H17" s="39" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="17" spans="8:11" x14ac:dyDescent="0.2">
-      <c r="H17" s="20" t="s">
+      <c r="I17" s="17" t="s">
         <v>23</v>
       </c>
-      <c r="I17" s="21" t="s">
+      <c r="J17" s="18">
+        <v>54</v>
+      </c>
+      <c r="K17" s="19">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="18" spans="8:11" x14ac:dyDescent="0.2">
+      <c r="H18" s="40"/>
+      <c r="I18" s="20" t="s">
         <v>24</v>
       </c>
-      <c r="J17" s="22">
-        <v>54</v>
-      </c>
-      <c r="K17" s="23">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="18" spans="8:11" x14ac:dyDescent="0.2">
-      <c r="H18" s="24"/>
-      <c r="I18" s="25" t="s">
+      <c r="J18" s="21" t="s">
         <v>25</v>
       </c>
-      <c r="J18" s="26" t="s">
+      <c r="K18" s="22" t="s">
         <v>26</v>
       </c>
-      <c r="K18" s="27" t="s">
+    </row>
+    <row r="19" spans="8:11" x14ac:dyDescent="0.2">
+      <c r="H19" s="40"/>
+      <c r="I19" s="23" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="19" spans="8:11" x14ac:dyDescent="0.2">
-      <c r="H19" s="24"/>
-      <c r="I19" s="28" t="s">
+      <c r="J19" s="21" t="s">
         <v>28</v>
       </c>
-      <c r="J19" s="26" t="s">
+      <c r="K19" s="22" t="s">
         <v>29</v>
       </c>
-      <c r="K19" s="27" t="s">
+    </row>
+    <row r="20" spans="8:11" x14ac:dyDescent="0.2">
+      <c r="H20" s="40"/>
+      <c r="I20" s="24" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="20" spans="8:11" x14ac:dyDescent="0.2">
-      <c r="H20" s="24"/>
-      <c r="I20" s="29" t="s">
+      <c r="J20" s="21" t="s">
         <v>31</v>
       </c>
-      <c r="J20" s="26" t="s">
+      <c r="K20" s="22" t="s">
         <v>32</v>
       </c>
-      <c r="K20" s="27" t="s">
+    </row>
+    <row r="21" spans="8:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="H21" s="41"/>
+      <c r="I21" s="25" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="21" spans="8:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="H21" s="30"/>
-      <c r="I21" s="31" t="s">
+      <c r="J21" s="26" t="s">
         <v>34</v>
       </c>
-      <c r="J21" s="32" t="s">
+      <c r="K21" s="27" t="s">
         <v>35</v>
       </c>
-      <c r="K21" s="33" t="s">
+    </row>
+    <row r="22" spans="8:11" x14ac:dyDescent="0.2">
+      <c r="H22" s="39" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="22" spans="8:11" x14ac:dyDescent="0.2">
-      <c r="H22" s="20" t="s">
+      <c r="I22" s="17" t="s">
+        <v>23</v>
+      </c>
+      <c r="J22" s="18">
+        <v>36</v>
+      </c>
+      <c r="K22" s="19">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="23" spans="8:11" x14ac:dyDescent="0.2">
+      <c r="H23" s="40"/>
+      <c r="I23" s="20" t="s">
+        <v>24</v>
+      </c>
+      <c r="J23" s="21" t="s">
         <v>37</v>
       </c>
-      <c r="I22" s="21" t="s">
+      <c r="K23" s="22">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="24" spans="8:11" x14ac:dyDescent="0.2">
+      <c r="H24" s="40"/>
+      <c r="I24" s="23" t="s">
+        <v>27</v>
+      </c>
+      <c r="J24" s="21" t="s">
+        <v>38</v>
+      </c>
+      <c r="K24" s="28">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="25" spans="8:11" x14ac:dyDescent="0.2">
+      <c r="H25" s="40"/>
+      <c r="I25" s="24" t="s">
+        <v>30</v>
+      </c>
+      <c r="J25" s="21" t="s">
+        <v>39</v>
+      </c>
+      <c r="K25" s="28">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="26" spans="8:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="H26" s="41"/>
+      <c r="I26" s="25" t="s">
+        <v>33</v>
+      </c>
+      <c r="J26" s="26" t="s">
+        <v>40</v>
+      </c>
+      <c r="K26" s="27">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="8:11" x14ac:dyDescent="0.2">
+      <c r="H27" s="39" t="s">
+        <v>41</v>
+      </c>
+      <c r="I27" s="17" t="s">
+        <v>23</v>
+      </c>
+      <c r="J27" s="29">
+        <v>10</v>
+      </c>
+      <c r="K27" s="19">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="28" spans="8:11" x14ac:dyDescent="0.2">
+      <c r="H28" s="40"/>
+      <c r="I28" s="20" t="s">
         <v>24</v>
       </c>
-      <c r="J22" s="22">
-        <v>36</v>
-      </c>
-      <c r="K22" s="23">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="23" spans="8:11" x14ac:dyDescent="0.2">
-      <c r="H23" s="24"/>
-      <c r="I23" s="25" t="s">
-        <v>25</v>
-      </c>
-      <c r="J23" s="26" t="s">
-        <v>38</v>
-      </c>
-      <c r="K23" s="27">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="24" spans="8:11" x14ac:dyDescent="0.2">
-      <c r="H24" s="24"/>
-      <c r="I24" s="28" t="s">
-        <v>28</v>
-      </c>
-      <c r="J24" s="26" t="s">
-        <v>39</v>
-      </c>
-      <c r="K24" s="34">
+      <c r="J28" s="21" t="s">
+        <v>42</v>
+      </c>
+      <c r="K28" s="22" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="29" spans="8:11" x14ac:dyDescent="0.2">
+      <c r="H29" s="40"/>
+      <c r="I29" s="23" t="s">
+        <v>27</v>
+      </c>
+      <c r="J29" s="30">
+        <v>10</v>
+      </c>
+      <c r="K29" s="31">
         <v>12</v>
       </c>
     </row>
-    <row r="25" spans="8:11" x14ac:dyDescent="0.2">
-      <c r="H25" s="24"/>
-      <c r="I25" s="29" t="s">
-        <v>31</v>
-      </c>
-      <c r="J25" s="26" t="s">
-        <v>40</v>
-      </c>
-      <c r="K25" s="34">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="26" spans="8:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="H26" s="30"/>
-      <c r="I26" s="31" t="s">
-        <v>34</v>
-      </c>
-      <c r="J26" s="32" t="s">
-        <v>41</v>
-      </c>
-      <c r="K26" s="33">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" spans="8:11" x14ac:dyDescent="0.2">
-      <c r="H27" s="20" t="s">
+    <row r="30" spans="8:11" x14ac:dyDescent="0.2">
+      <c r="H30" s="40"/>
+      <c r="I30" s="24" t="s">
+        <v>30</v>
+      </c>
+      <c r="J30" s="30">
+        <v>5</v>
+      </c>
+      <c r="K30" s="31">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="31" spans="8:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="H31" s="41"/>
+      <c r="I31" s="25" t="s">
+        <v>33</v>
+      </c>
+      <c r="J31" s="32">
+        <v>0</v>
+      </c>
+      <c r="K31" s="33">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="8:11" x14ac:dyDescent="0.2">
+      <c r="H32" s="42" t="s">
+        <v>43</v>
+      </c>
+      <c r="I32" s="17" t="s">
+        <v>23</v>
+      </c>
+      <c r="J32" s="29">
+        <v>14</v>
+      </c>
+      <c r="K32" s="34">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="33" spans="8:11" x14ac:dyDescent="0.2">
+      <c r="H33" s="43"/>
+      <c r="I33" s="20" t="s">
+        <v>24</v>
+      </c>
+      <c r="J33" s="21" t="s">
         <v>42</v>
       </c>
-      <c r="I27" s="21" t="s">
+      <c r="K33" s="22" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="34" spans="8:11" x14ac:dyDescent="0.2">
+      <c r="H34" s="43"/>
+      <c r="I34" s="23" t="s">
+        <v>27</v>
+      </c>
+      <c r="J34" s="30" t="s">
+        <v>44</v>
+      </c>
+      <c r="K34" s="31" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="35" spans="8:11" x14ac:dyDescent="0.2">
+      <c r="H35" s="43"/>
+      <c r="I35" s="24" t="s">
+        <v>30</v>
+      </c>
+      <c r="J35" s="30">
+        <v>2</v>
+      </c>
+      <c r="K35" s="31">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="36" spans="8:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="H36" s="44"/>
+      <c r="I36" s="25" t="s">
+        <v>33</v>
+      </c>
+      <c r="J36" s="32">
+        <v>0</v>
+      </c>
+      <c r="K36" s="33">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="8:11" x14ac:dyDescent="0.2">
+      <c r="H37" s="36" t="s">
+        <v>45</v>
+      </c>
+      <c r="I37" s="35" t="s">
         <v>24</v>
       </c>
-      <c r="J27" s="35">
-        <v>10</v>
-      </c>
-      <c r="K27" s="23">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="28" spans="8:11" x14ac:dyDescent="0.2">
-      <c r="H28" s="24"/>
-      <c r="I28" s="25" t="s">
-        <v>25</v>
-      </c>
-      <c r="J28" s="26" t="s">
-        <v>43</v>
-      </c>
-      <c r="K28" s="27" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="29" spans="8:11" x14ac:dyDescent="0.2">
-      <c r="H29" s="24"/>
-      <c r="I29" s="28" t="s">
-        <v>28</v>
-      </c>
-      <c r="J29" s="36">
-        <v>10</v>
-      </c>
-      <c r="K29" s="37">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="30" spans="8:11" x14ac:dyDescent="0.2">
-      <c r="H30" s="24"/>
-      <c r="I30" s="29" t="s">
-        <v>31</v>
-      </c>
-      <c r="J30" s="36">
-        <v>5</v>
-      </c>
-      <c r="K30" s="37">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="31" spans="8:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="H31" s="30"/>
-      <c r="I31" s="31" t="s">
-        <v>34</v>
-      </c>
-      <c r="J31" s="38">
-        <v>0</v>
-      </c>
-      <c r="K31" s="39">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="32" spans="8:11" x14ac:dyDescent="0.2">
-      <c r="H32" s="40" t="s">
-        <v>44</v>
-      </c>
-      <c r="I32" s="21" t="s">
-        <v>24</v>
-      </c>
-      <c r="J32" s="35">
-        <v>14</v>
-      </c>
-      <c r="K32" s="41">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="33" spans="8:11" x14ac:dyDescent="0.2">
-      <c r="H33" s="42"/>
-      <c r="I33" s="25" t="s">
-        <v>25</v>
-      </c>
-      <c r="J33" s="26" t="s">
-        <v>43</v>
-      </c>
-      <c r="K33" s="27" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="34" spans="8:11" x14ac:dyDescent="0.2">
-      <c r="H34" s="42"/>
-      <c r="I34" s="28" t="s">
-        <v>28</v>
-      </c>
-      <c r="J34" s="36" t="s">
-        <v>45</v>
-      </c>
-      <c r="K34" s="37" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="35" spans="8:11" x14ac:dyDescent="0.2">
-      <c r="H35" s="42"/>
-      <c r="I35" s="29" t="s">
-        <v>31</v>
-      </c>
-      <c r="J35" s="36">
-        <v>2</v>
-      </c>
-      <c r="K35" s="37">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="36" spans="8:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="H36" s="43"/>
-      <c r="I36" s="31" t="s">
-        <v>34</v>
-      </c>
-      <c r="J36" s="38">
-        <v>0</v>
-      </c>
-      <c r="K36" s="39">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="37" spans="8:11" x14ac:dyDescent="0.2">
-      <c r="H37" s="44" t="s">
+      <c r="J37" s="29" t="s">
         <v>46</v>
       </c>
-      <c r="I37" s="45" t="s">
-        <v>25</v>
-      </c>
-      <c r="J37" s="35" t="s">
+      <c r="K37" s="34" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="38" spans="8:11" x14ac:dyDescent="0.2">
+      <c r="H38" s="37"/>
+      <c r="I38" s="23" t="s">
+        <v>27</v>
+      </c>
+      <c r="J38" s="30" t="s">
         <v>47</v>
       </c>
-      <c r="K37" s="41" t="s">
+      <c r="K38" s="31" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="38" spans="8:11" x14ac:dyDescent="0.2">
-      <c r="H38" s="46"/>
-      <c r="I38" s="28" t="s">
-        <v>28</v>
-      </c>
-      <c r="J38" s="36" t="s">
+    <row r="39" spans="8:11" x14ac:dyDescent="0.2">
+      <c r="H39" s="37"/>
+      <c r="I39" s="24" t="s">
+        <v>30</v>
+      </c>
+      <c r="J39" s="30" t="s">
         <v>48</v>
       </c>
-      <c r="K38" s="37" t="s">
+      <c r="K39" s="31" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="39" spans="8:11" x14ac:dyDescent="0.2">
-      <c r="H39" s="46"/>
-      <c r="I39" s="29" t="s">
-        <v>31</v>
-      </c>
-      <c r="J39" s="36" t="s">
+    <row r="40" spans="8:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="H40" s="38"/>
+      <c r="I40" s="25" t="s">
+        <v>33</v>
+      </c>
+      <c r="J40" s="32" t="s">
         <v>49</v>
       </c>
-      <c r="K39" s="37" t="s">
+      <c r="K40" s="33" t="s">
         <v>49</v>
-      </c>
-    </row>
-    <row r="40" spans="8:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="H40" s="47"/>
-      <c r="I40" s="31" t="s">
-        <v>34</v>
-      </c>
-      <c r="J40" s="38" t="s">
-        <v>50</v>
-      </c>
-      <c r="K40" s="39" t="s">
-        <v>50</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="6">
+    <mergeCell ref="A8:E8"/>
     <mergeCell ref="H37:H40"/>
     <mergeCell ref="H17:H21"/>
     <mergeCell ref="H22:H26"/>
     <mergeCell ref="H27:H31"/>
     <mergeCell ref="H32:H36"/>
-    <mergeCell ref="A8:E8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1425,8 +1425,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{82FE0BB4-AF07-D248-8277-AD8E94C85802}">
   <dimension ref="A1:F11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1440,7 +1440,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C1" t="s">
         <v>1</v>
@@ -1497,7 +1497,7 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>16</v>
+        <v>50</v>
       </c>
       <c r="B4" t="b">
         <v>1</v>
@@ -1517,7 +1517,7 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>16</v>
+        <v>50</v>
       </c>
       <c r="B5" t="b">
         <v>0</v>
@@ -1537,7 +1537,7 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B6" t="b">
         <v>1</v>
@@ -1554,7 +1554,7 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B7" t="b">
         <v>0</v>
@@ -1571,7 +1571,7 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B8" t="b">
         <v>1</v>
@@ -1588,7 +1588,7 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B9" t="b">
         <v>0</v>
@@ -1605,7 +1605,7 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B10" t="b">
         <v>1</v>
@@ -1625,7 +1625,7 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B11" t="b">
         <v>0</v>

</xml_diff>

<commit_message>
feat: corrección de etiquetas en español y tab de perfil general de riesgo ahora tiene una pestaña por cada componente.
</commit_message>
<xml_diff>
--- a/src/R/risk_cut_offs.xlsx
+++ b/src/R/risk_cut_offs.xlsx
@@ -1,20 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11028"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11127"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/olivermazariegos/Sites/polio-risk/src/R/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CCDDDDC8-8A2D-4748-9315-CD46F6724E21}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2130697D-5267-FA46-BBC8-B56D5280EFA0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1900" yWindow="1820" windowWidth="24500" windowHeight="17240" activeTab="1" xr2:uid="{5C1FCA5E-1AE1-4E42-BC50-0F3DA39A67C4}"/>
+    <workbookView xWindow="1900" yWindow="1820" windowWidth="24500" windowHeight="17240" xr2:uid="{5C1FCA5E-1AE1-4E42-BC50-0F3DA39A67C4}"/>
   </bookViews>
   <sheets>
-    <sheet name="CUT OFFS" sheetId="1" r:id="rId1"/>
-    <sheet name="sheet_cut_off" sheetId="2" r:id="rId2"/>
+    <sheet name="sheet_cut_off" sheetId="2" r:id="rId1"/>
+    <sheet name="CUT OFFS" sheetId="1" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -590,6 +590,15 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -616,15 +625,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -939,489 +939,6 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F1957B83-55DF-0B40-AC0F-FC36128368F5}">
-  <dimension ref="A1:K40"/>
-  <sheetViews>
-    <sheetView topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="D30" sqref="D30"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="5" width="17.83203125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A1" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="6" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A2" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="B2" s="1"/>
-      <c r="C2" s="1"/>
-      <c r="D2" s="1"/>
-      <c r="E2" s="1"/>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A3" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" s="1"/>
-      <c r="C3" s="1"/>
-      <c r="D3" s="1"/>
-      <c r="E3" s="1"/>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A4" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="B4" s="1"/>
-      <c r="C4" s="1"/>
-      <c r="D4" s="1"/>
-      <c r="E4" s="1"/>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A5" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="B5" s="1"/>
-      <c r="C5" s="1"/>
-      <c r="D5" s="1"/>
-      <c r="E5" s="1"/>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A6" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="B6" s="1">
-        <v>34</v>
-      </c>
-      <c r="C6" s="1">
-        <v>48</v>
-      </c>
-      <c r="D6" s="1">
-        <v>60</v>
-      </c>
-      <c r="E6" s="1">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A8" s="45" t="s">
-        <v>10</v>
-      </c>
-      <c r="B8" s="46"/>
-      <c r="C8" s="46"/>
-      <c r="D8" s="46"/>
-      <c r="E8" s="47"/>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A9" s="8" t="s">
-        <v>0</v>
-      </c>
-      <c r="B9" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C9" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="D9" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="E9" s="9" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A10" s="10" t="s">
-        <v>5</v>
-      </c>
-      <c r="B10" s="7"/>
-      <c r="C10" s="7"/>
-      <c r="D10" s="7"/>
-      <c r="E10" s="11"/>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A11" s="10" t="s">
-        <v>6</v>
-      </c>
-      <c r="B11" s="7"/>
-      <c r="C11" s="7"/>
-      <c r="D11" s="7"/>
-      <c r="E11" s="11"/>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A12" s="10" t="s">
-        <v>7</v>
-      </c>
-      <c r="B12" s="7"/>
-      <c r="C12" s="7"/>
-      <c r="D12" s="7"/>
-      <c r="E12" s="11"/>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A13" s="10" t="s">
-        <v>8</v>
-      </c>
-      <c r="B13" s="7"/>
-      <c r="C13" s="7"/>
-      <c r="D13" s="7"/>
-      <c r="E13" s="11"/>
-    </row>
-    <row r="14" spans="1:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="12" t="s">
-        <v>9</v>
-      </c>
-      <c r="B14" s="13" t="s">
-        <v>11</v>
-      </c>
-      <c r="C14" s="13" t="s">
-        <v>12</v>
-      </c>
-      <c r="D14" s="13" t="s">
-        <v>13</v>
-      </c>
-      <c r="E14" s="14" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="16" spans="1:11" ht="120" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="I16" s="15"/>
-      <c r="J16" s="16" t="s">
-        <v>20</v>
-      </c>
-      <c r="K16" s="16" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="17" spans="8:11" x14ac:dyDescent="0.2">
-      <c r="H17" s="39" t="s">
-        <v>22</v>
-      </c>
-      <c r="I17" s="17" t="s">
-        <v>23</v>
-      </c>
-      <c r="J17" s="18">
-        <v>54</v>
-      </c>
-      <c r="K17" s="19">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="18" spans="8:11" x14ac:dyDescent="0.2">
-      <c r="H18" s="40"/>
-      <c r="I18" s="20" t="s">
-        <v>24</v>
-      </c>
-      <c r="J18" s="21" t="s">
-        <v>25</v>
-      </c>
-      <c r="K18" s="22" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="19" spans="8:11" x14ac:dyDescent="0.2">
-      <c r="H19" s="40"/>
-      <c r="I19" s="23" t="s">
-        <v>27</v>
-      </c>
-      <c r="J19" s="21" t="s">
-        <v>28</v>
-      </c>
-      <c r="K19" s="22" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="20" spans="8:11" x14ac:dyDescent="0.2">
-      <c r="H20" s="40"/>
-      <c r="I20" s="24" t="s">
-        <v>30</v>
-      </c>
-      <c r="J20" s="21" t="s">
-        <v>31</v>
-      </c>
-      <c r="K20" s="22" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="21" spans="8:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="H21" s="41"/>
-      <c r="I21" s="25" t="s">
-        <v>33</v>
-      </c>
-      <c r="J21" s="26" t="s">
-        <v>34</v>
-      </c>
-      <c r="K21" s="27" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="22" spans="8:11" x14ac:dyDescent="0.2">
-      <c r="H22" s="39" t="s">
-        <v>36</v>
-      </c>
-      <c r="I22" s="17" t="s">
-        <v>23</v>
-      </c>
-      <c r="J22" s="18">
-        <v>36</v>
-      </c>
-      <c r="K22" s="19">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="23" spans="8:11" x14ac:dyDescent="0.2">
-      <c r="H23" s="40"/>
-      <c r="I23" s="20" t="s">
-        <v>24</v>
-      </c>
-      <c r="J23" s="21" t="s">
-        <v>37</v>
-      </c>
-      <c r="K23" s="22">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="24" spans="8:11" x14ac:dyDescent="0.2">
-      <c r="H24" s="40"/>
-      <c r="I24" s="23" t="s">
-        <v>27</v>
-      </c>
-      <c r="J24" s="21" t="s">
-        <v>38</v>
-      </c>
-      <c r="K24" s="28">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="25" spans="8:11" x14ac:dyDescent="0.2">
-      <c r="H25" s="40"/>
-      <c r="I25" s="24" t="s">
-        <v>30</v>
-      </c>
-      <c r="J25" s="21" t="s">
-        <v>39</v>
-      </c>
-      <c r="K25" s="28">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="26" spans="8:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="H26" s="41"/>
-      <c r="I26" s="25" t="s">
-        <v>33</v>
-      </c>
-      <c r="J26" s="26" t="s">
-        <v>40</v>
-      </c>
-      <c r="K26" s="27">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" spans="8:11" x14ac:dyDescent="0.2">
-      <c r="H27" s="39" t="s">
-        <v>41</v>
-      </c>
-      <c r="I27" s="17" t="s">
-        <v>23</v>
-      </c>
-      <c r="J27" s="29">
-        <v>10</v>
-      </c>
-      <c r="K27" s="19">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="28" spans="8:11" x14ac:dyDescent="0.2">
-      <c r="H28" s="40"/>
-      <c r="I28" s="20" t="s">
-        <v>24</v>
-      </c>
-      <c r="J28" s="21" t="s">
-        <v>42</v>
-      </c>
-      <c r="K28" s="22" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="29" spans="8:11" x14ac:dyDescent="0.2">
-      <c r="H29" s="40"/>
-      <c r="I29" s="23" t="s">
-        <v>27</v>
-      </c>
-      <c r="J29" s="30">
-        <v>10</v>
-      </c>
-      <c r="K29" s="31">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="30" spans="8:11" x14ac:dyDescent="0.2">
-      <c r="H30" s="40"/>
-      <c r="I30" s="24" t="s">
-        <v>30</v>
-      </c>
-      <c r="J30" s="30">
-        <v>5</v>
-      </c>
-      <c r="K30" s="31">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="31" spans="8:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="H31" s="41"/>
-      <c r="I31" s="25" t="s">
-        <v>33</v>
-      </c>
-      <c r="J31" s="32">
-        <v>0</v>
-      </c>
-      <c r="K31" s="33">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="32" spans="8:11" x14ac:dyDescent="0.2">
-      <c r="H32" s="42" t="s">
-        <v>43</v>
-      </c>
-      <c r="I32" s="17" t="s">
-        <v>23</v>
-      </c>
-      <c r="J32" s="29">
-        <v>14</v>
-      </c>
-      <c r="K32" s="34">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="33" spans="8:11" x14ac:dyDescent="0.2">
-      <c r="H33" s="43"/>
-      <c r="I33" s="20" t="s">
-        <v>24</v>
-      </c>
-      <c r="J33" s="21" t="s">
-        <v>42</v>
-      </c>
-      <c r="K33" s="22" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="34" spans="8:11" x14ac:dyDescent="0.2">
-      <c r="H34" s="43"/>
-      <c r="I34" s="23" t="s">
-        <v>27</v>
-      </c>
-      <c r="J34" s="30" t="s">
-        <v>44</v>
-      </c>
-      <c r="K34" s="31" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="35" spans="8:11" x14ac:dyDescent="0.2">
-      <c r="H35" s="43"/>
-      <c r="I35" s="24" t="s">
-        <v>30</v>
-      </c>
-      <c r="J35" s="30">
-        <v>2</v>
-      </c>
-      <c r="K35" s="31">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="36" spans="8:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="H36" s="44"/>
-      <c r="I36" s="25" t="s">
-        <v>33</v>
-      </c>
-      <c r="J36" s="32">
-        <v>0</v>
-      </c>
-      <c r="K36" s="33">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="37" spans="8:11" x14ac:dyDescent="0.2">
-      <c r="H37" s="36" t="s">
-        <v>45</v>
-      </c>
-      <c r="I37" s="35" t="s">
-        <v>24</v>
-      </c>
-      <c r="J37" s="29" t="s">
-        <v>46</v>
-      </c>
-      <c r="K37" s="34" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="38" spans="8:11" x14ac:dyDescent="0.2">
-      <c r="H38" s="37"/>
-      <c r="I38" s="23" t="s">
-        <v>27</v>
-      </c>
-      <c r="J38" s="30" t="s">
-        <v>47</v>
-      </c>
-      <c r="K38" s="31" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="39" spans="8:11" x14ac:dyDescent="0.2">
-      <c r="H39" s="37"/>
-      <c r="I39" s="24" t="s">
-        <v>30</v>
-      </c>
-      <c r="J39" s="30" t="s">
-        <v>48</v>
-      </c>
-      <c r="K39" s="31" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="40" spans="8:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="H40" s="38"/>
-      <c r="I40" s="25" t="s">
-        <v>33</v>
-      </c>
-      <c r="J40" s="32" t="s">
-        <v>49</v>
-      </c>
-      <c r="K40" s="33" t="s">
-        <v>49</v>
-      </c>
-    </row>
-  </sheetData>
-  <mergeCells count="6">
-    <mergeCell ref="A8:E8"/>
-    <mergeCell ref="H37:H40"/>
-    <mergeCell ref="H17:H21"/>
-    <mergeCell ref="H22:H26"/>
-    <mergeCell ref="H27:H31"/>
-    <mergeCell ref="H32:H36"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{82FE0BB4-AF07-D248-8277-AD8E94C85802}">
   <dimension ref="A1:F11"/>
   <sheetViews>
@@ -1646,4 +1163,487 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F1957B83-55DF-0B40-AC0F-FC36128368F5}">
+  <dimension ref="A1:K40"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="5" width="17.83203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="6" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A2" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="1"/>
+      <c r="C2" s="1"/>
+      <c r="D2" s="1"/>
+      <c r="E2" s="1"/>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A3" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="1"/>
+      <c r="C3" s="1"/>
+      <c r="D3" s="1"/>
+      <c r="E3" s="1"/>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A4" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" s="1"/>
+      <c r="C4" s="1"/>
+      <c r="D4" s="1"/>
+      <c r="E4" s="1"/>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A5" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" s="1"/>
+      <c r="C5" s="1"/>
+      <c r="D5" s="1"/>
+      <c r="E5" s="1"/>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A6" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" s="1">
+        <v>34</v>
+      </c>
+      <c r="C6" s="1">
+        <v>48</v>
+      </c>
+      <c r="D6" s="1">
+        <v>60</v>
+      </c>
+      <c r="E6" s="1">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A8" s="36" t="s">
+        <v>10</v>
+      </c>
+      <c r="B8" s="37"/>
+      <c r="C8" s="37"/>
+      <c r="D8" s="37"/>
+      <c r="E8" s="38"/>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A9" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="E9" s="9" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A10" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="B10" s="7"/>
+      <c r="C10" s="7"/>
+      <c r="D10" s="7"/>
+      <c r="E10" s="11"/>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A11" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="B11" s="7"/>
+      <c r="C11" s="7"/>
+      <c r="D11" s="7"/>
+      <c r="E11" s="11"/>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A12" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="B12" s="7"/>
+      <c r="C12" s="7"/>
+      <c r="D12" s="7"/>
+      <c r="E12" s="11"/>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A13" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="B13" s="7"/>
+      <c r="C13" s="7"/>
+      <c r="D13" s="7"/>
+      <c r="E13" s="11"/>
+    </row>
+    <row r="14" spans="1:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="B14" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="C14" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="D14" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="E14" s="14" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" ht="120" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="I16" s="15"/>
+      <c r="J16" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="K16" s="16" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="17" spans="8:11" x14ac:dyDescent="0.2">
+      <c r="H17" s="42" t="s">
+        <v>22</v>
+      </c>
+      <c r="I17" s="17" t="s">
+        <v>23</v>
+      </c>
+      <c r="J17" s="18">
+        <v>54</v>
+      </c>
+      <c r="K17" s="19">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="18" spans="8:11" x14ac:dyDescent="0.2">
+      <c r="H18" s="43"/>
+      <c r="I18" s="20" t="s">
+        <v>24</v>
+      </c>
+      <c r="J18" s="21" t="s">
+        <v>25</v>
+      </c>
+      <c r="K18" s="22" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="19" spans="8:11" x14ac:dyDescent="0.2">
+      <c r="H19" s="43"/>
+      <c r="I19" s="23" t="s">
+        <v>27</v>
+      </c>
+      <c r="J19" s="21" t="s">
+        <v>28</v>
+      </c>
+      <c r="K19" s="22" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="20" spans="8:11" x14ac:dyDescent="0.2">
+      <c r="H20" s="43"/>
+      <c r="I20" s="24" t="s">
+        <v>30</v>
+      </c>
+      <c r="J20" s="21" t="s">
+        <v>31</v>
+      </c>
+      <c r="K20" s="22" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="21" spans="8:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="H21" s="44"/>
+      <c r="I21" s="25" t="s">
+        <v>33</v>
+      </c>
+      <c r="J21" s="26" t="s">
+        <v>34</v>
+      </c>
+      <c r="K21" s="27" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="22" spans="8:11" x14ac:dyDescent="0.2">
+      <c r="H22" s="42" t="s">
+        <v>36</v>
+      </c>
+      <c r="I22" s="17" t="s">
+        <v>23</v>
+      </c>
+      <c r="J22" s="18">
+        <v>36</v>
+      </c>
+      <c r="K22" s="19">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="23" spans="8:11" x14ac:dyDescent="0.2">
+      <c r="H23" s="43"/>
+      <c r="I23" s="20" t="s">
+        <v>24</v>
+      </c>
+      <c r="J23" s="21" t="s">
+        <v>37</v>
+      </c>
+      <c r="K23" s="22">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="24" spans="8:11" x14ac:dyDescent="0.2">
+      <c r="H24" s="43"/>
+      <c r="I24" s="23" t="s">
+        <v>27</v>
+      </c>
+      <c r="J24" s="21" t="s">
+        <v>38</v>
+      </c>
+      <c r="K24" s="28">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="25" spans="8:11" x14ac:dyDescent="0.2">
+      <c r="H25" s="43"/>
+      <c r="I25" s="24" t="s">
+        <v>30</v>
+      </c>
+      <c r="J25" s="21" t="s">
+        <v>39</v>
+      </c>
+      <c r="K25" s="28">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="26" spans="8:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="H26" s="44"/>
+      <c r="I26" s="25" t="s">
+        <v>33</v>
+      </c>
+      <c r="J26" s="26" t="s">
+        <v>40</v>
+      </c>
+      <c r="K26" s="27">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="8:11" x14ac:dyDescent="0.2">
+      <c r="H27" s="42" t="s">
+        <v>41</v>
+      </c>
+      <c r="I27" s="17" t="s">
+        <v>23</v>
+      </c>
+      <c r="J27" s="29">
+        <v>10</v>
+      </c>
+      <c r="K27" s="19">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="28" spans="8:11" x14ac:dyDescent="0.2">
+      <c r="H28" s="43"/>
+      <c r="I28" s="20" t="s">
+        <v>24</v>
+      </c>
+      <c r="J28" s="21" t="s">
+        <v>42</v>
+      </c>
+      <c r="K28" s="22" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="29" spans="8:11" x14ac:dyDescent="0.2">
+      <c r="H29" s="43"/>
+      <c r="I29" s="23" t="s">
+        <v>27</v>
+      </c>
+      <c r="J29" s="30">
+        <v>10</v>
+      </c>
+      <c r="K29" s="31">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="30" spans="8:11" x14ac:dyDescent="0.2">
+      <c r="H30" s="43"/>
+      <c r="I30" s="24" t="s">
+        <v>30</v>
+      </c>
+      <c r="J30" s="30">
+        <v>5</v>
+      </c>
+      <c r="K30" s="31">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="31" spans="8:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="H31" s="44"/>
+      <c r="I31" s="25" t="s">
+        <v>33</v>
+      </c>
+      <c r="J31" s="32">
+        <v>0</v>
+      </c>
+      <c r="K31" s="33">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="8:11" x14ac:dyDescent="0.2">
+      <c r="H32" s="45" t="s">
+        <v>43</v>
+      </c>
+      <c r="I32" s="17" t="s">
+        <v>23</v>
+      </c>
+      <c r="J32" s="29">
+        <v>14</v>
+      </c>
+      <c r="K32" s="34">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="33" spans="8:11" x14ac:dyDescent="0.2">
+      <c r="H33" s="46"/>
+      <c r="I33" s="20" t="s">
+        <v>24</v>
+      </c>
+      <c r="J33" s="21" t="s">
+        <v>42</v>
+      </c>
+      <c r="K33" s="22" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="34" spans="8:11" x14ac:dyDescent="0.2">
+      <c r="H34" s="46"/>
+      <c r="I34" s="23" t="s">
+        <v>27</v>
+      </c>
+      <c r="J34" s="30" t="s">
+        <v>44</v>
+      </c>
+      <c r="K34" s="31" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="35" spans="8:11" x14ac:dyDescent="0.2">
+      <c r="H35" s="46"/>
+      <c r="I35" s="24" t="s">
+        <v>30</v>
+      </c>
+      <c r="J35" s="30">
+        <v>2</v>
+      </c>
+      <c r="K35" s="31">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="36" spans="8:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="H36" s="47"/>
+      <c r="I36" s="25" t="s">
+        <v>33</v>
+      </c>
+      <c r="J36" s="32">
+        <v>0</v>
+      </c>
+      <c r="K36" s="33">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="8:11" x14ac:dyDescent="0.2">
+      <c r="H37" s="39" t="s">
+        <v>45</v>
+      </c>
+      <c r="I37" s="35" t="s">
+        <v>24</v>
+      </c>
+      <c r="J37" s="29" t="s">
+        <v>46</v>
+      </c>
+      <c r="K37" s="34" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="38" spans="8:11" x14ac:dyDescent="0.2">
+      <c r="H38" s="40"/>
+      <c r="I38" s="23" t="s">
+        <v>27</v>
+      </c>
+      <c r="J38" s="30" t="s">
+        <v>47</v>
+      </c>
+      <c r="K38" s="31" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="39" spans="8:11" x14ac:dyDescent="0.2">
+      <c r="H39" s="40"/>
+      <c r="I39" s="24" t="s">
+        <v>30</v>
+      </c>
+      <c r="J39" s="30" t="s">
+        <v>48</v>
+      </c>
+      <c r="K39" s="31" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="40" spans="8:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="H40" s="41"/>
+      <c r="I40" s="25" t="s">
+        <v>33</v>
+      </c>
+      <c r="J40" s="32" t="s">
+        <v>49</v>
+      </c>
+      <c r="K40" s="33" t="s">
+        <v>49</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="6">
+    <mergeCell ref="A8:E8"/>
+    <mergeCell ref="H37:H40"/>
+    <mergeCell ref="H17:H21"/>
+    <mergeCell ref="H22:H26"/>
+    <mergeCell ref="H27:H31"/>
+    <mergeCell ref="H32:H36"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>